<commit_message>
fixed super checking on startup
</commit_message>
<xml_diff>
--- a/nControl Tracker.xlsx
+++ b/nControl Tracker.xlsx
@@ -61,9 +61,6 @@
     <t>ACTIVITY</t>
   </si>
   <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
     <t>Activity 02</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>nControl</t>
+  </si>
+  <si>
+    <t>Login: Shared Prefs</t>
   </si>
 </sst>
 </file>
@@ -956,13 +956,13 @@
   <dimension ref="B2:BQ34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
@@ -972,7 +972,7 @@
   <sheetData>
     <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -988,7 +988,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="I3" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1008,11 +1008,11 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -1020,7 +1020,7 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="14"/>
       <c r="AL3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1282,13 +1282,13 @@
     </row>
     <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
       </c>
       <c r="D9" s="16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="16">
         <v>1</v>
@@ -1297,12 +1297,12 @@
         <v>4</v>
       </c>
       <c r="G9" s="17">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="16">
         <v>2</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="16">
         <v>4</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="16">
         <v>4</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="16">
         <v>4</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="16">
         <v>5</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="16">
         <v>5</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="16">
         <v>5</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="16">
         <v>6</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="18">
         <v>6</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="16">
         <v>9</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="16">
         <v>9</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="16">
         <v>9</v>
@@ -1562,7 +1562,7 @@
     </row>
     <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="16">
         <v>9</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="16">
         <v>10</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="16">
         <v>11</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="16">
         <v>12</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="16">
         <v>12</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="16">
         <v>14</v>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="16">
         <v>14</v>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="16">
         <v>14</v>
@@ -1722,7 +1722,7 @@
     </row>
     <row r="31" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="16">
         <v>15</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="32" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="16">
         <v>15</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="16">
         <v>15</v>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="16">
         <v>16</v>

</xml_diff>